<commit_message>
update 20 Abril (faltan distritos)
</commit_message>
<xml_diff>
--- a/datos/test_Andalucia.xlsx
+++ b/datos/test_Andalucia.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +970,29 @@
         <v>0.15220385674931131</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43940</v>
+      </c>
+      <c r="B26">
+        <v>48527</v>
+      </c>
+      <c r="C26">
+        <v>11555</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26" si="3">B26-B25</f>
+        <v>457</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26" si="4">C26-C25</f>
+        <v>130</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26" si="5">E26/D26</f>
+        <v>0.28446389496717722</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add datos municipios 7 Mayo (aun no añadidos a csv gral de municipios)
</commit_message>
<xml_diff>
--- a/datos/test_Andalucia.xlsx
+++ b/datos/test_Andalucia.xlsx
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:F42"/>
+      <selection activeCell="D42" sqref="D42:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,6 +1361,29 @@
         <v>0.36567164179104478</v>
       </c>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B43">
+        <v>61432</v>
+      </c>
+      <c r="C43">
+        <v>14870</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43" si="54">B43-B42</f>
+        <v>555</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ref="E43" si="55">C43-C42</f>
+        <v>231</v>
+      </c>
+      <c r="F43">
+        <f t="shared" ref="F43" si="56">E43/D43</f>
+        <v>0.41621621621621624</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>